<commit_message>
Rollover fix + 4096 Size
Yas
</commit_message>
<xml_diff>
--- a/Throughputs Graphs.xlsx
+++ b/Throughputs Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hungn\OneDrive\Documents\GitHub\RingSTM-with-Ring-Rollover-and-RingSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{266D417D-E6FE-4763-AC22-5C2AD68C48C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{4F84EC79-562E-4421-A5E1-AB9736FCFB30}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{266D417D-E6FE-4763-AC22-5C2AD68C48C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{4FB1BEFA-E397-4D98-813E-2B9BE6FC77BB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10928" xr2:uid="{73835AD5-ACCD-4A8F-9A15-186238187320}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Bloom Filter Size: 1024</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Commit/Aborts</t>
+  </si>
+  <si>
+    <t>Bloom Filter Size: 4096</t>
   </si>
 </sst>
 </file>
@@ -207,8 +210,66 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4096</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.8132700000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.211541</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80962400000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6021-4C40-8962-586B210B4CDB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>1024</c:v>
           </c:tx>
@@ -224,7 +285,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -242,18 +303,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:f>Sheet1!$B$16:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.1159209999999999</c:v>
+                  <c:v>1.148501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50858700000000001</c:v>
+                  <c:v>0.56208999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38784000000000002</c:v>
+                  <c:v>0.40609099999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -266,7 +327,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>256</c:v>
           </c:tx>
@@ -282,7 +343,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -300,18 +361,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$18</c:f>
+              <c:f>Sheet1!$B$28:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0022979999999999</c:v>
+                  <c:v>1.0022960000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40355400000000002</c:v>
+                  <c:v>0.38168800000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31828600000000001</c:v>
+                  <c:v>0.31145099999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -324,7 +385,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>64</c:v>
           </c:tx>
@@ -338,20 +399,38 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$B$30</c:f>
+              <c:f>Sheet1!$A$40:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0010950000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40232899999999999</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35384399999999999</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$40:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0032909999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39814699999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28902499999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,7 +607,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Commits</a:t>
+                  <a:t>Commits/Aborts</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -755,8 +834,66 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4096</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60173</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109280</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26AB-4A66-A3EA-7EFA943DEE43}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>1024</c:v>
           </c:tx>
@@ -772,7 +909,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -790,7 +927,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$11</c:f>
+              <c:f>Sheet1!$B$21:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -814,7 +951,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>256</c:v>
           </c:tx>
@@ -830,7 +967,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -848,7 +985,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$B$23</c:f>
+              <c:f>Sheet1!$B$33:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -872,7 +1009,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>64</c:v>
           </c:tx>
@@ -886,9 +1023,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$9:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$B$35</c:f>
+              <c:f>Sheet1!$B$45:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2311,16 +2466,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>347672</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>138116</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>642948</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>71441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2349,16 +2504,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>80962</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>42863</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>423862</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>314334</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66679</xdr:rowOff>
+      <xdr:colOff>9534</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>147642</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2388,22 +2543,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114298</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>103227</xdr:rowOff>
+      <xdr:colOff>100011</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>411941</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>46077</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>311098</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9C01C4F-AF46-40E3-A108-A3AAC22E0651}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2877C08-929B-4E8E-96D4-86E92364EE48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2419,8 +2574,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="114298" y="9532977"/>
-          <a:ext cx="7603318" cy="4572000"/>
+          <a:off x="100011" y="20640675"/>
+          <a:ext cx="4925962" cy="3657600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2431,23 +2586,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>187728</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>232175</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81C847F2-90B7-4AEE-A38B-83EE52FA15D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4E81908-67A2-4C95-884A-0A37A6F239E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2463,8 +2618,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7419975" y="9525001"/>
-          <a:ext cx="7845828" cy="4572000"/>
+          <a:off x="95250" y="16654462"/>
+          <a:ext cx="4851800" cy="3657600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2475,23 +2630,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>80964</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>61913</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>145150</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>298217</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5AECDD7-4342-44AD-8DC7-A91E5C180C69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C28BC1C5-251B-46D6-93B1-80EBFF9B5E51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2507,8 +2662,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15287625" y="9510712"/>
-          <a:ext cx="7708000" cy="4572000"/>
+          <a:off x="80964" y="12749213"/>
+          <a:ext cx="4932128" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>138113</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361294</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45272900-3A7A-465C-9DE7-53FF75C7D87B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="138113" y="6767513"/>
+          <a:ext cx="4938056" cy="3657600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2817,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CD40C5-B010-4D95-8E2E-6A0BC3AB4020}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -2832,7 +3031,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -2853,7 +3052,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>1.1159209999999999</v>
+        <v>2.8132700000000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2861,7 +3060,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>0.50858700000000001</v>
+        <v>1.211541</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2869,7 +3068,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0.38784000000000002</v>
+        <v>0.80962400000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2888,7 +3087,7 @@
         <v>60173</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -2905,17 +3104,17 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="8"/>
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2926,24 +3125,24 @@
       <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B16" s="5">
-        <v>1.0022979999999999</v>
+      <c r="B16" s="2">
+        <v>1.148501</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
-        <v>0.40355400000000002</v>
+      <c r="B17" s="2">
+        <v>0.56208999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>8</v>
       </c>
-      <c r="B18" s="5">
-        <v>0.31828600000000001</v>
+      <c r="B18" s="2">
+        <v>0.40609099999999998</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -2959,15 +3158,15 @@
         <v>2</v>
       </c>
       <c r="B21" s="5">
-        <v>56614</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>60173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>4</v>
       </c>
       <c r="B22" s="5">
-        <v>103842</v>
+        <v>109280</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -2975,14 +3174,14 @@
         <v>8</v>
       </c>
       <c r="B23" s="5">
-        <v>88128</v>
+        <v>96801</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="7"/>
+      <c r="A25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="8"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -3001,7 +3200,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="5">
-        <v>1.0010950000000001</v>
+        <v>1.0022960000000001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -3009,7 +3208,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="5">
-        <v>0.40232899999999999</v>
+        <v>0.38168800000000003</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -3017,7 +3216,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="5">
-        <v>0.35384399999999999</v>
+        <v>0.31145099999999998</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -3033,7 +3232,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="5">
-        <v>51066</v>
+        <v>56614</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -3041,7 +3240,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="5">
-        <v>90371</v>
+        <v>103842</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -3049,14 +3248,109 @@
         <v>8</v>
       </c>
       <c r="B35" s="5">
+        <v>88128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>2</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1.0032909999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>4</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0.39814699999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>8</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.28902499999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>2</v>
+      </c>
+      <c r="B45" s="5">
+        <v>51066</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>4</v>
+      </c>
+      <c r="B46" s="5">
+        <v>90371</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>8</v>
+      </c>
+      <c r="B47" s="5">
         <v>70909</v>
       </c>
     </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" s="1">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>